<commit_message>
Store roles need do combo next
</commit_message>
<xml_diff>
--- a/prefixes.xlsx
+++ b/prefixes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="431">
   <si>
     <t>ID</t>
   </si>
@@ -47,6 +47,87 @@
     <t>Last Updated</t>
   </si>
   <si>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/100/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/100/</t>
+  </si>
+  <si>
+    <t>10.16.11.0/24</t>
+  </si>
+  <si>
+    <t>IPv4</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2024-10-10T05:51:16.635888Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T05:51:16.635929Z</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/97/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/97/</t>
+  </si>
+  <si>
+    <t>10.16.16.0/24</t>
+  </si>
+  <si>
+    <t>2024-10-10T05:37:21.290205Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T05:37:21.290251Z</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/98/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/98/</t>
+  </si>
+  <si>
+    <t>10.16.22.0/24</t>
+  </si>
+  <si>
+    <t>2024-10-10T05:40:38.561113Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T05:40:38.561142Z</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/99/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/99/</t>
+  </si>
+  <si>
+    <t>10.16.89.0/24</t>
+  </si>
+  <si>
+    <t>2024-10-10T05:42:15.730154Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T05:42:15.730186Z</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/96/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/96/</t>
+  </si>
+  <si>
+    <t>10.16.99.0/24</t>
+  </si>
+  <si>
+    <t>2024-10-10T05:19:11.329263Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T05:19:11.329296Z</t>
+  </si>
+  <si>
     <t>https://demo.netbox.dev/api/ipam/prefixes/1/</t>
   </si>
   <si>
@@ -56,9 +137,6 @@
     <t>10.112.0.0/15</t>
   </si>
   <si>
-    <t>IPv4</t>
-  </si>
-  <si>
     <t>Dunder-Mifflin, Inc.</t>
   </si>
   <si>
@@ -872,24 +950,6 @@
     <t>2020-12-30T20:13:45.870000Z</t>
   </si>
   <si>
-    <t>https://demo.netbox.dev/api/ipam/prefixes/96/</t>
-  </si>
-  <si>
-    <t>https://demo.netbox.dev/ipam/prefixes/96/</t>
-  </si>
-  <si>
-    <t>10.128.36.0/24</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>2024-10-09T06:22:46.274822Z</t>
-  </si>
-  <si>
-    <t>2024-10-09T06:22:46.274861Z</t>
-  </si>
-  <si>
     <t>https://demo.netbox.dev/api/ipam/prefixes/73/</t>
   </si>
   <si>
@@ -905,19 +965,97 @@
     <t>2021-12-30T16:35:35.870000Z</t>
   </si>
   <si>
-    <t>https://demo.netbox.dev/api/ipam/prefixes/97/</t>
-  </si>
-  <si>
-    <t>https://demo.netbox.dev/ipam/prefixes/97/</t>
-  </si>
-  <si>
-    <t>29.220.191.254/32</t>
-  </si>
-  <si>
-    <t>2024-10-09T08:08:57.630028Z</t>
-  </si>
-  <si>
-    <t>2024-10-09T08:14:30.113778Z</t>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/107/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/107/</t>
+  </si>
+  <si>
+    <t>192.168.11.0/24</t>
+  </si>
+  <si>
+    <t>R00</t>
+  </si>
+  <si>
+    <t>2024-10-10T08:45:36.971466Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T09:31:38.480618Z</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/108/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/108/</t>
+  </si>
+  <si>
+    <t>192.168.12.0/24</t>
+  </si>
+  <si>
+    <t>2024-10-10T08:45:37.040249Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T09:31:47.529738Z</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/109/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/109/</t>
+  </si>
+  <si>
+    <t>192.168.13.0/24</t>
+  </si>
+  <si>
+    <t>2024-10-10T08:45:37.103183Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T09:31:56.309818Z</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/110/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/110/</t>
+  </si>
+  <si>
+    <t>192.168.14.0/24</t>
+  </si>
+  <si>
+    <t>2024-10-10T08:45:37.186221Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T09:27:26.645937Z</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/111/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/111/</t>
+  </si>
+  <si>
+    <t>192.168.15.0/24</t>
+  </si>
+  <si>
+    <t>2024-10-10T08:45:37.266636Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T09:27:50.181664Z</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/api/ipam/prefixes/112/</t>
+  </si>
+  <si>
+    <t>https://demo.netbox.dev/ipam/prefixes/112/</t>
+  </si>
+  <si>
+    <t>192.168.16.0/24</t>
+  </si>
+  <si>
+    <t>2024-10-10T08:45:37.331323Z</t>
+  </si>
+  <si>
+    <t>2024-10-10T09:27:59.886744Z</t>
   </si>
   <si>
     <t>https://demo.netbox.dev/api/ipam/prefixes/75/</t>
@@ -966,18 +1104,6 @@
   </si>
   <si>
     <t>2022-04-08T00:17:07.610000Z</t>
-  </si>
-  <si>
-    <t>https://demo.netbox.dev/api/ipam/prefixes/98/</t>
-  </si>
-  <si>
-    <t>https://demo.netbox.dev/ipam/prefixes/98/</t>
-  </si>
-  <si>
-    <t>2024-10-09T08:10:35.431809Z</t>
-  </si>
-  <si>
-    <t>2024-10-09T08:10:35.431846Z</t>
   </si>
   <si>
     <t>https://demo.netbox.dev/api/ipam/prefixes/76/</t>
@@ -1535,7 +1661,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1567,7 +1693,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -1591,24 +1717,24 @@
         <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1617,30 +1743,30 @@
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1649,30 +1775,30 @@
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1681,30 +1807,30 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -1713,30 +1839,30 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -1745,30 +1871,30 @@
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -1777,30 +1903,30 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I9" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -1809,30 +1935,30 @@
         <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J10" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -1841,30 +1967,30 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I11" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J11" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1873,30 +1999,30 @@
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I12" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -1905,30 +2031,30 @@
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I13" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -1937,30 +2063,30 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I14" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J14" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1969,30 +2095,30 @@
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H15" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I15" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J15" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -2001,30 +2127,30 @@
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H16" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I16" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J16" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -2033,30 +2159,30 @@
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H17" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I17" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J17" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -2065,30 +2191,30 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I18" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J18" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -2097,30 +2223,30 @@
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="H19" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I19" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J19" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -2129,30 +2255,30 @@
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H20" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I20" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J20" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E21">
         <v>4</v>
@@ -2161,30 +2287,30 @@
         <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H21" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I21" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J21" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -2193,30 +2319,30 @@
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="H22" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I22" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J22" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -2225,30 +2351,30 @@
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="H23" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I23" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J23" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -2257,30 +2383,30 @@
         <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="H24" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I24" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J24" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D25" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -2289,30 +2415,30 @@
         <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="H25" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I25" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J25" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D26" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -2321,30 +2447,30 @@
         <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H26" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I26" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J26" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -2353,30 +2479,30 @@
         <v>13</v>
       </c>
       <c r="G27" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="H27" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I27" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J27" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C28" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D28" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -2385,30 +2511,30 @@
         <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="H28" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I28" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J28" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -2417,30 +2543,30 @@
         <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H29" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I29" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J29" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D30" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E30">
         <v>4</v>
@@ -2449,30 +2575,30 @@
         <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H30" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I30" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J30" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C31" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -2481,30 +2607,30 @@
         <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="H31" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I31" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J31" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C32" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D32" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -2513,30 +2639,30 @@
         <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H32" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I32" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J32" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C33" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D33" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -2545,30 +2671,30 @@
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H33" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I33" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J33" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D34" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -2577,30 +2703,30 @@
         <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="H34" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I34" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J34" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C35" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D35" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E35">
         <v>4</v>
@@ -2609,30 +2735,30 @@
         <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="H35" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I35" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J35" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C36" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D36" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -2641,30 +2767,30 @@
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H36" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I36" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J36" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C37" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -2673,30 +2799,30 @@
         <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H37" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I37" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J37" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C38" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -2705,30 +2831,30 @@
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="H38" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I38" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J38" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D39" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -2737,30 +2863,30 @@
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="H39" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I39" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J39" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C40" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D40" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="E40">
         <v>4</v>
@@ -2769,30 +2895,30 @@
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="H40" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I40" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J40" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B41" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C41" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D41" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -2801,30 +2927,30 @@
         <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H41" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I41" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J41" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C42" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D42" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="E42">
         <v>4</v>
@@ -2833,30 +2959,30 @@
         <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H42" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I42" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J42" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B43" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C43" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="E43">
         <v>4</v>
@@ -2865,30 +2991,30 @@
         <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="H43" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I43" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J43" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B44" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C44" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D44" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E44">
         <v>4</v>
@@ -2897,30 +3023,30 @@
         <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="H44" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I44" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J44" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C45" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="D45" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="E45">
         <v>4</v>
@@ -2929,30 +3055,30 @@
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="H45" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I45" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J45" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C46" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D46" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -2961,30 +3087,30 @@
         <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="H46" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I46" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J46" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C47" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D47" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="E47">
         <v>4</v>
@@ -2993,30 +3119,30 @@
         <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="H47" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I47" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J47" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C48" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D48" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="E48">
         <v>4</v>
@@ -3025,30 +3151,30 @@
         <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="H48" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I48" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J48" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C49" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D49" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E49">
         <v>4</v>
@@ -3057,30 +3183,30 @@
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="H49" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I49" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J49" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C50" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D50" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E50">
         <v>4</v>
@@ -3089,30 +3215,30 @@
         <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="H50" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I50" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J50" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C51" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D51" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E51">
         <v>4</v>
@@ -3121,30 +3247,30 @@
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="H51" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I51" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J51" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C52" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D52" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -3153,30 +3279,30 @@
         <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="H52" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I52" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J52" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B53" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C53" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D53" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="E53">
         <v>4</v>
@@ -3185,30 +3311,30 @@
         <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="H53" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I53" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J53" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C54" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="D54" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -3217,30 +3343,30 @@
         <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="H54" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I54" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J54" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C55" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="D55" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="E55">
         <v>4</v>
@@ -3249,30 +3375,30 @@
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="H55" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I55" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J55" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C56" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="D56" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="E56">
         <v>4</v>
@@ -3281,30 +3407,30 @@
         <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="H56" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I56" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J56" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C57" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="D57" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -3313,30 +3439,30 @@
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="H57" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I57" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J57" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C58" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="D58" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E58">
         <v>4</v>
@@ -3345,30 +3471,30 @@
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H58" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I58" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J58" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B59" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C59" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D59" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E59">
         <v>4</v>
@@ -3377,30 +3503,30 @@
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="H59" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I59" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J59" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C60" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D60" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="E60">
         <v>4</v>
@@ -3409,30 +3535,30 @@
         <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="H60" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I60" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J60" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B61" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C61" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="D61" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="E61">
         <v>4</v>
@@ -3441,30 +3567,30 @@
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="H61" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I61" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J61" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B62" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="C62" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D62" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="E62">
         <v>4</v>
@@ -3473,30 +3599,30 @@
         <v>13</v>
       </c>
       <c r="G62" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="H62" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I62" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J62" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B63" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C63" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="D63" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="E63">
         <v>4</v>
@@ -3505,30 +3631,30 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="H63" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I63" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J63" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B64" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C64" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="D64" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="E64">
         <v>4</v>
@@ -3537,30 +3663,30 @@
         <v>13</v>
       </c>
       <c r="G64" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="H64" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I64" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J64" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C65" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="D65" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="E65">
         <v>4</v>
@@ -3569,30 +3695,30 @@
         <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="H65" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I65" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J65" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B66" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C66" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="D66" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="E66">
         <v>4</v>
@@ -3601,30 +3727,30 @@
         <v>13</v>
       </c>
       <c r="G66" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="H66" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I66" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J66" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B67" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C67" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="D67" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="E67">
         <v>4</v>
@@ -3633,30 +3759,30 @@
         <v>13</v>
       </c>
       <c r="G67" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="H67" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I67" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J67" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B68" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C68" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="D68" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="E68">
         <v>4</v>
@@ -3665,30 +3791,30 @@
         <v>13</v>
       </c>
       <c r="G68" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="H68" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I68" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J68" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B69" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="C69" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="D69" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="E69">
         <v>4</v>
@@ -3697,30 +3823,30 @@
         <v>13</v>
       </c>
       <c r="G69" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="H69" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I69" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="J69" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C70" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="D70" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="E70">
         <v>4</v>
@@ -3729,30 +3855,30 @@
         <v>13</v>
       </c>
       <c r="G70" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="H70" t="s">
-        <v>288</v>
+        <v>40</v>
       </c>
       <c r="I70" t="s">
-        <v>289</v>
+        <v>41</v>
       </c>
       <c r="J70" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B71" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C71" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D71" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="E71">
         <v>4</v>
@@ -3761,30 +3887,30 @@
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="H71" t="s">
-        <v>288</v>
+        <v>40</v>
       </c>
       <c r="I71" t="s">
-        <v>294</v>
+        <v>41</v>
       </c>
       <c r="J71" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="B72" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C72" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D72" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E72">
         <v>4</v>
@@ -3793,30 +3919,30 @@
         <v>13</v>
       </c>
       <c r="G72" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="H72" t="s">
-        <v>288</v>
+        <v>40</v>
       </c>
       <c r="I72" t="s">
-        <v>299</v>
+        <v>41</v>
       </c>
       <c r="J72" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B73" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C73" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D73" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E73">
         <v>4</v>
@@ -3825,30 +3951,30 @@
         <v>13</v>
       </c>
       <c r="G73" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H73" t="s">
-        <v>288</v>
+        <v>40</v>
       </c>
       <c r="I73" t="s">
-        <v>304</v>
+        <v>41</v>
       </c>
       <c r="J73" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C74" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D74" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E74">
         <v>4</v>
@@ -3857,30 +3983,30 @@
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H74" t="s">
-        <v>288</v>
+        <v>40</v>
       </c>
       <c r="I74" t="s">
-        <v>308</v>
+        <v>41</v>
       </c>
       <c r="J74" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C75" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D75" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E75">
         <v>4</v>
@@ -3889,30 +4015,30 @@
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="H75" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I75" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="J75" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="B76" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C76" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D76" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E76">
         <v>4</v>
@@ -3921,30 +4047,30 @@
         <v>13</v>
       </c>
       <c r="G76" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="H76" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="I76" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="J76" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B77" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C77" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D77" t="s">
-        <v>298</v>
+        <v>324</v>
       </c>
       <c r="E77">
         <v>4</v>
@@ -3953,30 +4079,30 @@
         <v>13</v>
       </c>
       <c r="G77" t="s">
-        <v>298</v>
+        <v>324</v>
       </c>
       <c r="H77" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="I77" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="J77" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="B78" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="C78" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="D78" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="E78">
         <v>4</v>
@@ -3985,30 +4111,30 @@
         <v>13</v>
       </c>
       <c r="G78" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="H78" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="I78" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="J78" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="B79" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C79" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="D79" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="E79">
         <v>4</v>
@@ -4017,30 +4143,30 @@
         <v>13</v>
       </c>
       <c r="G79" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="H79" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="I79" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="J79" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="B80" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="C80" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="D80" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="E80">
         <v>4</v>
@@ -4049,30 +4175,30 @@
         <v>13</v>
       </c>
       <c r="G80" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="H80" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="I80" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="J80" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="B81" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="C81" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="D81" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="E81">
         <v>4</v>
@@ -4081,30 +4207,30 @@
         <v>13</v>
       </c>
       <c r="G81" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="H81" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="I81" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="J81" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B82" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="C82" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="D82" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="E82">
         <v>4</v>
@@ -4113,30 +4239,30 @@
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="H82" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I82" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="J82" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B83" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="C83" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="D83" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="E83">
         <v>4</v>
@@ -4145,30 +4271,30 @@
         <v>13</v>
       </c>
       <c r="G83" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="H83" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I83" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="J83" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="C84" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="D84" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="E84">
         <v>4</v>
@@ -4177,30 +4303,30 @@
         <v>13</v>
       </c>
       <c r="G84" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="H84" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I84" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="J84" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="C85" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="D85" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="E85">
         <v>4</v>
@@ -4209,30 +4335,30 @@
         <v>13</v>
       </c>
       <c r="G85" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="H85" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I85" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="J85" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B86" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="C86" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="D86" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="E86">
         <v>4</v>
@@ -4241,30 +4367,30 @@
         <v>13</v>
       </c>
       <c r="G86" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="H86" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I86" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="J86" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="C87" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="D87" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="E87">
         <v>4</v>
@@ -4273,30 +4399,30 @@
         <v>13</v>
       </c>
       <c r="G87" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="H87" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I87" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="J87" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B88" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="C88" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="D88" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="E88">
         <v>4</v>
@@ -4305,30 +4431,30 @@
         <v>13</v>
       </c>
       <c r="G88" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="H88" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I88" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="J88" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B89" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="C89" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="D89" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="E89">
         <v>4</v>
@@ -4337,30 +4463,30 @@
         <v>13</v>
       </c>
       <c r="G89" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="H89" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I89" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="J89" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B90" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="C90" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="D90" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="E90">
         <v>4</v>
@@ -4369,30 +4495,30 @@
         <v>13</v>
       </c>
       <c r="G90" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="H90" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I90" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="J90" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="C91" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="D91" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="E91">
         <v>4</v>
@@ -4401,30 +4527,30 @@
         <v>13</v>
       </c>
       <c r="G91" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="H91" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I91" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="J91" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B92" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="C92" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="D92" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="E92">
         <v>4</v>
@@ -4433,30 +4559,30 @@
         <v>13</v>
       </c>
       <c r="G92" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="H92" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I92" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="J92" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="C93" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="D93" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="E93">
         <v>4</v>
@@ -4465,48 +4591,304 @@
         <v>13</v>
       </c>
       <c r="G93" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="H93" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="I93" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="J93" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
+        <v>78</v>
+      </c>
+      <c r="B94" t="s">
+        <v>395</v>
+      </c>
+      <c r="C94" t="s">
+        <v>396</v>
+      </c>
+      <c r="D94" t="s">
+        <v>397</v>
+      </c>
+      <c r="E94">
+        <v>4</v>
+      </c>
+      <c r="F94" t="s">
+        <v>13</v>
+      </c>
+      <c r="G94" t="s">
+        <v>397</v>
+      </c>
+      <c r="H94" t="s">
+        <v>14</v>
+      </c>
+      <c r="I94" t="s">
+        <v>398</v>
+      </c>
+      <c r="J94" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>89</v>
+      </c>
+      <c r="B95" t="s">
+        <v>399</v>
+      </c>
+      <c r="C95" t="s">
+        <v>400</v>
+      </c>
+      <c r="D95" t="s">
+        <v>401</v>
+      </c>
+      <c r="E95">
+        <v>4</v>
+      </c>
+      <c r="F95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95" t="s">
+        <v>401</v>
+      </c>
+      <c r="H95" t="s">
+        <v>14</v>
+      </c>
+      <c r="I95" t="s">
+        <v>402</v>
+      </c>
+      <c r="J95" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>90</v>
+      </c>
+      <c r="B96" t="s">
+        <v>403</v>
+      </c>
+      <c r="C96" t="s">
+        <v>404</v>
+      </c>
+      <c r="D96" t="s">
+        <v>405</v>
+      </c>
+      <c r="E96">
+        <v>4</v>
+      </c>
+      <c r="F96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G96" t="s">
+        <v>405</v>
+      </c>
+      <c r="H96" t="s">
+        <v>14</v>
+      </c>
+      <c r="I96" t="s">
+        <v>406</v>
+      </c>
+      <c r="J96" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>91</v>
+      </c>
+      <c r="B97" t="s">
+        <v>407</v>
+      </c>
+      <c r="C97" t="s">
+        <v>408</v>
+      </c>
+      <c r="D97" t="s">
+        <v>409</v>
+      </c>
+      <c r="E97">
+        <v>4</v>
+      </c>
+      <c r="F97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G97" t="s">
+        <v>409</v>
+      </c>
+      <c r="H97" t="s">
+        <v>14</v>
+      </c>
+      <c r="I97" t="s">
+        <v>410</v>
+      </c>
+      <c r="J97" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>79</v>
+      </c>
+      <c r="B98" t="s">
+        <v>411</v>
+      </c>
+      <c r="C98" t="s">
+        <v>412</v>
+      </c>
+      <c r="D98" t="s">
+        <v>413</v>
+      </c>
+      <c r="E98">
+        <v>4</v>
+      </c>
+      <c r="F98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98" t="s">
+        <v>413</v>
+      </c>
+      <c r="H98" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" t="s">
+        <v>414</v>
+      </c>
+      <c r="J98" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99">
+        <v>92</v>
+      </c>
+      <c r="B99" t="s">
+        <v>415</v>
+      </c>
+      <c r="C99" t="s">
+        <v>416</v>
+      </c>
+      <c r="D99" t="s">
+        <v>417</v>
+      </c>
+      <c r="E99">
+        <v>4</v>
+      </c>
+      <c r="F99" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" t="s">
+        <v>417</v>
+      </c>
+      <c r="H99" t="s">
+        <v>14</v>
+      </c>
+      <c r="I99" t="s">
+        <v>418</v>
+      </c>
+      <c r="J99" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>93</v>
+      </c>
+      <c r="B100" t="s">
+        <v>419</v>
+      </c>
+      <c r="C100" t="s">
+        <v>420</v>
+      </c>
+      <c r="D100" t="s">
+        <v>421</v>
+      </c>
+      <c r="E100">
+        <v>4</v>
+      </c>
+      <c r="F100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100" t="s">
+        <v>421</v>
+      </c>
+      <c r="H100" t="s">
+        <v>14</v>
+      </c>
+      <c r="I100" t="s">
+        <v>422</v>
+      </c>
+      <c r="J100" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>94</v>
+      </c>
+      <c r="B101" t="s">
+        <v>423</v>
+      </c>
+      <c r="C101" t="s">
+        <v>424</v>
+      </c>
+      <c r="D101" t="s">
+        <v>425</v>
+      </c>
+      <c r="E101">
+        <v>4</v>
+      </c>
+      <c r="F101" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101" t="s">
+        <v>425</v>
+      </c>
+      <c r="H101" t="s">
+        <v>14</v>
+      </c>
+      <c r="I101" t="s">
+        <v>426</v>
+      </c>
+      <c r="J101" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102">
         <v>95</v>
       </c>
-      <c r="B94" t="s">
-        <v>385</v>
-      </c>
-      <c r="C94" t="s">
-        <v>386</v>
-      </c>
-      <c r="D94" t="s">
-        <v>387</v>
-      </c>
-      <c r="E94">
-        <v>4</v>
-      </c>
-      <c r="F94" t="s">
-        <v>13</v>
-      </c>
-      <c r="G94" t="s">
-        <v>387</v>
-      </c>
-      <c r="H94" t="s">
-        <v>288</v>
-      </c>
-      <c r="I94" t="s">
-        <v>388</v>
-      </c>
-      <c r="J94" t="s">
-        <v>388</v>
+      <c r="B102" t="s">
+        <v>427</v>
+      </c>
+      <c r="C102" t="s">
+        <v>428</v>
+      </c>
+      <c r="D102" t="s">
+        <v>429</v>
+      </c>
+      <c r="E102">
+        <v>4</v>
+      </c>
+      <c r="F102" t="s">
+        <v>13</v>
+      </c>
+      <c r="G102" t="s">
+        <v>429</v>
+      </c>
+      <c r="H102" t="s">
+        <v>14</v>
+      </c>
+      <c r="I102" t="s">
+        <v>430</v>
+      </c>
+      <c r="J102" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>